<commit_message>
Final report sent at 24/05/2021
</commit_message>
<xml_diff>
--- a/data/processed/dados.xlsx
+++ b/data/processed/dados.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dados_originais" sheetId="1" state="visible" r:id="rId2"/>
@@ -739,7 +739,7 @@
       <selection pane="topLeft" activeCell="BC1" activeCellId="0" sqref="BC1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="1" style="0" width="19.99"/>
   </cols>
@@ -1922,11 +1922,11 @@
   </sheetPr>
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2290,7 +2290,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2650,11 +2650,11 @@
   </sheetPr>
   <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3018,7 +3018,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="84.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.57"/>

</xml_diff>